<commit_message>
test run after major changes
</commit_message>
<xml_diff>
--- a/new2.xlsx
+++ b/new2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E91"/>
+  <dimension ref="A1:F91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,11 @@
           <t>Artists</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Plays  May 11, 2025</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -486,6 +491,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>1841991</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -513,6 +523,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>49152</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -540,6 +555,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>123928</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -567,6 +587,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>505808</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -594,6 +619,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>102997</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -621,6 +651,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>5690</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -648,6 +683,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>66632</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -675,6 +715,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>30722</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -702,6 +747,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>15535</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -727,6 +777,11 @@
       <c r="E11" t="inlineStr">
         <is>
           <t>Armonian</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>72591</t>
         </is>
       </c>
     </row>
@@ -752,6 +807,11 @@
           <t>Invalid URL</t>
         </is>
       </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Invalid URL</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -779,6 +839,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>57556</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -806,6 +871,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>62694</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -833,6 +903,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>32419</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -860,6 +935,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>85842</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -887,6 +967,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>15303</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -912,6 +997,11 @@
       <c r="E18" t="inlineStr">
         <is>
           <t>Armonian</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>9810</t>
         </is>
       </c>
     </row>
@@ -937,6 +1027,11 @@
           <t>Invalid URL</t>
         </is>
       </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Invalid URL</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -964,6 +1059,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>98292</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -991,6 +1091,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>5879</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1018,6 +1123,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>5347</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1045,6 +1155,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>10386</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1072,6 +1187,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>7145</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1099,6 +1219,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>45358</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1126,6 +1251,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>28824</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1153,6 +1283,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>17721</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1180,6 +1315,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>20523</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1207,6 +1347,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>105671</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1234,6 +1379,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>3685</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1261,6 +1411,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>17515</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1288,6 +1443,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>5003</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1315,6 +1475,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>6544</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1342,6 +1507,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>16523</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1369,6 +1539,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>19360</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1396,6 +1571,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>6594</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1423,6 +1603,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>52795</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1450,6 +1635,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>6050</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1477,6 +1667,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>4372</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1504,6 +1699,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>9913</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1531,6 +1731,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>21007</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1558,6 +1763,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>13773</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1585,6 +1795,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>11633</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1612,6 +1827,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>29316</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1639,6 +1859,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>8016</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1664,6 +1889,11 @@
       <c r="E46" t="inlineStr">
         <is>
           <t>Armonian</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>14177</t>
         </is>
       </c>
     </row>
@@ -1689,6 +1919,11 @@
           <t>Invalid URL</t>
         </is>
       </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Invalid URL</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1716,6 +1951,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>14092</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1743,6 +1983,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>26343</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1770,6 +2015,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>7259</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1797,6 +2047,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>3874</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1824,6 +2079,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>33175</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1851,6 +2111,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>7239</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1878,6 +2143,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>11638</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1905,6 +2175,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>17344</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1932,6 +2207,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>7351</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1959,6 +2239,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>15794</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1986,6 +2271,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>6086</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2013,6 +2303,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>23017</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2040,6 +2335,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>4929</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2067,6 +2367,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>10333</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2094,6 +2399,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>8828</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2121,6 +2431,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>9202</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2148,6 +2463,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>6446</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2175,6 +2495,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>9575</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2200,6 +2525,11 @@
       <c r="E66" t="inlineStr">
         <is>
           <t>Armonian</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>4672</t>
         </is>
       </c>
     </row>
@@ -2225,6 +2555,11 @@
           <t>Invalid URL</t>
         </is>
       </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Invalid URL</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2252,6 +2587,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>12193</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2279,6 +2619,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>5077</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2304,6 +2649,11 @@
       <c r="E70" t="inlineStr">
         <is>
           <t>Armonian</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>6353</t>
         </is>
       </c>
     </row>
@@ -2329,6 +2679,11 @@
           <t>Invalid URL</t>
         </is>
       </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>Invalid URL</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2356,6 +2711,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>1629</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2383,6 +2743,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>45358</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2410,6 +2775,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>105671</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2437,6 +2807,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>1150</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2464,6 +2839,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>14177</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -2491,6 +2871,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>3874</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -2518,6 +2903,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>29316</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -2545,6 +2935,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>1118</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -2572,6 +2967,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>4229</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -2599,6 +2999,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>5490</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -2626,6 +3031,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>2125</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -2653,6 +3063,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>2068</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -2680,6 +3095,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>2120</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -2707,6 +3127,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>1322</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -2734,6 +3159,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>27487</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -2761,6 +3191,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>416</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -2788,6 +3223,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>1161</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -2815,6 +3255,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>1061</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -2842,6 +3287,11 @@
           <t>Armonian</t>
         </is>
       </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>504</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -2867,6 +3317,11 @@
       <c r="E91" t="inlineStr">
         <is>
           <t>Armonian</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>1420</t>
         </is>
       </c>
     </row>

</xml_diff>